<commit_message>
Updated excel. Attempted stalls. Dying.
</commit_message>
<xml_diff>
--- a/Controls.xlsx
+++ b/Controls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
   <si>
     <t>MemRead</t>
   </si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t>043a</t>
-  </si>
-  <si>
-    <t>0521</t>
   </si>
   <si>
     <t>OpHex</t>
@@ -646,7 +643,7 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+      <selection activeCell="D16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,7 +668,7 @@
         <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
         <v>44</v>
@@ -736,7 +733,7 @@
         <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>45</v>
@@ -801,7 +798,7 @@
         <v>36</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3">
@@ -864,7 +861,7 @@
         <v>35</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>46</v>
@@ -929,7 +926,7 @@
         <v>37</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5">
@@ -983,7 +980,7 @@
         <v>35</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>48</v>
@@ -1039,7 +1036,7 @@
         <v>35</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>49</v>
@@ -1095,7 +1092,7 @@
         <v>38</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8">
@@ -1149,7 +1146,7 @@
         <v>35</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>47</v>
@@ -1205,7 +1202,7 @@
         <v>35</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>50</v>
@@ -1261,7 +1258,7 @@
         <v>39</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11">
@@ -1304,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="V11" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
@@ -1315,7 +1312,7 @@
         <v>40</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12">
@@ -1358,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="V12" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
@@ -1369,7 +1366,7 @@
         <v>41</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13">
@@ -1423,7 +1420,7 @@
         <v>42</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14">
@@ -1477,7 +1474,7 @@
         <v>43</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15">
@@ -1531,7 +1528,7 @@
         <v>35</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>36</v>
@@ -1543,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="9">
         <v>0</v>
@@ -1558,10 +1555,10 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="12">
         <v>0</v>
@@ -1575,8 +1572,8 @@
       <c r="U16" s="10">
         <v>1</v>
       </c>
-      <c r="V16" s="14" t="s">
-        <v>59</v>
+      <c r="V16" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="5:22" x14ac:dyDescent="0.3">
@@ -1587,7 +1584,7 @@
         <v>35</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>35</v>
@@ -1643,7 +1640,7 @@
         <v>35</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>42</v>

</xml_diff>